<commit_message>
Updated some data - poverty, labor, tax statistics
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BIR-Tax-Statistics.xlsx
+++ b/Data/Fiscal Data/BIR-Tax-Statistics.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19828010-1433-4F86-BD1A-2D40BDCCE601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A519DBD-4032-4473-8A0B-52E50C6C72CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1665" yWindow="4245" windowWidth="12810" windowHeight="10545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="By Source, Millions" sheetId="1" r:id="rId1"/>
-    <sheet name="metadata" sheetId="2" r:id="rId2"/>
+    <sheet name="Goals_RMO" sheetId="3" r:id="rId2"/>
+    <sheet name="metadata" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="324">
   <si>
     <t>Tax Classification</t>
   </si>
@@ -471,9 +472,6 @@
     <t>BIR Collections - Actual</t>
   </si>
   <si>
-    <t>Annual Reports 2008 - 2021</t>
-  </si>
-  <si>
     <t>BIR Collections - Goal</t>
   </si>
   <si>
@@ -505,17 +503,528 @@
   </si>
   <si>
     <t>2024 Goal</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>Annual Reports 2008 - 2023</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>RMO</t>
+  </si>
+  <si>
+    <t>IssueDate</t>
+  </si>
+  <si>
+    <t>TargetCY</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Goal_TotalRevenue</t>
+  </si>
+  <si>
+    <t>Goal_NetIncomeandProfits</t>
+  </si>
+  <si>
+    <t>Goal_ExciseTaxes</t>
+  </si>
+  <si>
+    <t>Goal_ValueAddedTaxes</t>
+  </si>
+  <si>
+    <t>Goal_PercentageTaxes</t>
+  </si>
+  <si>
+    <t>Goal_OtherTaxes</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/9637rmo11_tables%201-9.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 11-2002</t>
+  </si>
+  <si>
+    <t>May 10, 2002</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/4216rmo26_tbls.%201-9.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 26-2002</t>
+  </si>
+  <si>
+    <t>October 9, 2002</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/2357rmo03_20.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 20-2003</t>
+  </si>
+  <si>
+    <t>June 4, 2003</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>Initial/Final</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/1798rmo04_06tab1.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 6-2004</t>
+  </si>
+  <si>
+    <t>February 17, 2004</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/15713rmo05-02%20(tables).pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 2-2005</t>
+  </si>
+  <si>
+    <t>January 18, 2005</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/28330rmo06_06tables.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 6-2006</t>
+  </si>
+  <si>
+    <t>February 15, 2006</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/34743Tables.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 7-2007</t>
+  </si>
+  <si>
+    <t>April 27, 2007</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>RMO No. 17-2008</t>
+  </si>
+  <si>
+    <t>May 16, 2008</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>RMO No. 7-2009</t>
+  </si>
+  <si>
+    <t>April 6 , 2009</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>RMO No. 25-2009</t>
+  </si>
+  <si>
+    <t>July 9, 2009</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/50100Annexes_rmo_31-2010_revised_again.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 31-2010</t>
+  </si>
+  <si>
+    <t>March 24, 2010</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>RMO No. 66-2010</t>
+  </si>
+  <si>
+    <t>July 30, 2010</t>
+  </si>
+  <si>
+    <t>RMO No. 12-2011</t>
+  </si>
+  <si>
+    <t>March 17, 2011</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>RMO No. 1-2012</t>
+  </si>
+  <si>
+    <t>January 12, 2012</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>RMO No. 1-2013</t>
+  </si>
+  <si>
+    <t>January 24, 2013</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/81226Tables%20RMO%204-2014.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 4-2014</t>
+  </si>
+  <si>
+    <t>January 16, 2014</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>RMO No. 7-2014</t>
+  </si>
+  <si>
+    <t>January 24, 2014</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Full%20Text%20of%20RMO%202015/RMO%202%20Table%201.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 2-2015</t>
+  </si>
+  <si>
+    <t>January 13, 2015</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Full%20Text%20of%20RMO%202015/RMO%204%20Annexes%20Table%201%20to%205.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 4-2015</t>
+  </si>
+  <si>
+    <t>February 6, 2015</t>
+  </si>
+  <si>
+    <t>Revision 1</t>
+  </si>
+  <si>
+    <t>RMO No. 5-2015</t>
+  </si>
+  <si>
+    <t>March 12, 2015</t>
+  </si>
+  <si>
+    <t>RMO No. 2-2016</t>
+  </si>
+  <si>
+    <t>January 8, 2016</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>RMO No. 7-2017</t>
+  </si>
+  <si>
+    <t>March 16, 2017</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202018/Tables%201-4%20and%205A-5F.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 8-2018</t>
+  </si>
+  <si>
+    <t>January 29, 2018</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>RMO No. 10-2018</t>
+  </si>
+  <si>
+    <t>February 22, 2018</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202019/RMO%209-2019/RMO%209-2019%20Annexes.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 9-2019</t>
+  </si>
+  <si>
+    <t>February 11, 2019</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202019/Revised%20CY%202019%20BIR%20Goal_Tables%202-5F.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 18-2019</t>
+  </si>
+  <si>
+    <t>April 26, 2019</t>
+  </si>
+  <si>
+    <t>RMO No. 29-2019</t>
+  </si>
+  <si>
+    <t>June 6, 2019</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/RMO%202-2020%20Annexes.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 2-2020</t>
+  </si>
+  <si>
+    <t>January 16, 2020</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/RMO%20No.%2012-2020%20Annexes.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 12-2020</t>
+  </si>
+  <si>
+    <t>April 27, 2020</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/RMO%20Annexes_pdf.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 16-2020</t>
+  </si>
+  <si>
+    <t>June 16, 2020</t>
+  </si>
+  <si>
+    <t>Revision 2</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/Annexes_pdf.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 30-2020</t>
+  </si>
+  <si>
+    <t>September 22, 2020</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202021/RMO_No.%207-2021_Annexes_CY%202021%20GOAL.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 7-2021</t>
+  </si>
+  <si>
+    <t>February 2, 2021</t>
+  </si>
+  <si>
+    <t>RMO No. 27-2021</t>
+  </si>
+  <si>
+    <t>October 25, 2021</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Attachments/RMO16-2022_Annexes.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 16-2022</t>
+  </si>
+  <si>
+    <t>March 15, 2022</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Attachments/RMO%2030/RMO%20No.%2030-2022%20Table%205A-F.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 30-2022</t>
+  </si>
+  <si>
+    <t>June 9, 2022</t>
+  </si>
+  <si>
+    <t>RMO No. 53-2022</t>
+  </si>
+  <si>
+    <t>December 7, 2022</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2023/Full%20Text/CY2023_RMO%20Annexes_based%20on%20MTRP%20Dec.5%202022-BL.PDF</t>
+  </si>
+  <si>
+    <t>RMO No. 15-2023</t>
+  </si>
+  <si>
+    <t>April 25, 2023</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2023/RMO%20No.%2027-2023/Revised_CY2023_RMO%20Annexes%201.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 27-2023</t>
+  </si>
+  <si>
+    <t>July 27, 2023</t>
+  </si>
+  <si>
+    <t>RMO No. 34-2023</t>
+  </si>
+  <si>
+    <t>October 19, 2023</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/RMO%20No.%2011-2024%20Annexes.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 11-2024</t>
+  </si>
+  <si>
+    <t>March 14, 2024</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/CY2024%20Goal%20_RMO%2029-2024%20Annexes.xlsx</t>
+  </si>
+  <si>
+    <t>RMO No. 29-2024</t>
+  </si>
+  <si>
+    <t>July 22, 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.bir.gov.ph/revenue-memorandum-orders </t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/bir-archive</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/39979RMO%2017-2008%20Annexes.pdf</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/46675amended%20annexes%20of%20rmo%2025.PDF</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/45613Annexes_rmo7-09.pdf</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/52599RMO%2066-2010-Annexes.pdf</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/57045ANNEXES_for%20email.pdf</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/61827Copy%20of%20ANNEXES_RMO1-2012.pdf</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/68142Table1.pdf</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/81819Tables%20RMO%207-2014.pdf</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/RMO%20No.%205-2015%20Annexes%20Table%201%20to%205.pdf</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/RMO%20No.%202-2016%20Annexes%20Table%201%20to%205.pdf</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/RMO%207%20-%202017%20Tables.xlsx</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/local/pdf/Tables%201-4%20and%205A-5F_copy.pdf</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/RMO%2018-2019%20Revised%20CY%202019%20BIR%20Goal_Tables%202-5F.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 46-2020</t>
+  </si>
+  <si>
+    <t>December 23, 2020</t>
+  </si>
+  <si>
+    <t>Revision 3</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/local/pdf/Revised_RMO%2045_Annexes.pdf</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/local/pdf/RMO%20No.%2027-2021_Annexes.pdf</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/local/pdf/Revised%20CY2022%20RMO%20Goal%20Annexes.pdf</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/local/pdf/RMO%20No.%2034-2023%20Table%202%20to%205F.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -547,12 +1056,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -566,20 +1081,25 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -808,13 +1328,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CH47"/>
+  <dimension ref="A1:CH48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="L41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,16 +1359,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" t="s">
         <v>155</v>
       </c>
-      <c r="C1" t="s">
-        <v>156</v>
-      </c>
       <c r="D1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" t="s">
         <v>153</v>
-      </c>
-      <c r="E1" t="s">
-        <v>154</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -9353,6 +9873,17 @@
         <v>287.49</v>
       </c>
     </row>
+    <row r="48" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>26495.599999999999</v>
+      </c>
+      <c r="E48">
+        <v>24522.1</v>
+      </c>
+      <c r="G48">
+        <v>21672.799999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -9360,11 +9891,1549 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9F3864-6467-428D-BD82-6F0581A8CF64}">
+  <dimension ref="A1:K43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A38" sqref="A38"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="17.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="9" customWidth="1"/>
+    <col min="7" max="11" width="12.85546875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" s="9">
+        <v>447556</v>
+      </c>
+      <c r="G2" s="9">
+        <v>244966</v>
+      </c>
+      <c r="H2" s="9">
+        <v>66638</v>
+      </c>
+      <c r="I2" s="9">
+        <v>75929</v>
+      </c>
+      <c r="J2" s="9">
+        <v>35918</v>
+      </c>
+      <c r="K2" s="9">
+        <v>24105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" s="9">
+        <v>422516</v>
+      </c>
+      <c r="G3" s="9">
+        <v>243499</v>
+      </c>
+      <c r="H3" s="9">
+        <v>54600</v>
+      </c>
+      <c r="I3" s="9">
+        <v>68795</v>
+      </c>
+      <c r="J3" s="9">
+        <v>28812</v>
+      </c>
+      <c r="K3" s="9">
+        <v>26810</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" s="9">
+        <v>424007</v>
+      </c>
+      <c r="G4" s="9">
+        <v>242672</v>
+      </c>
+      <c r="H4" s="9">
+        <v>58406</v>
+      </c>
+      <c r="I4" s="9">
+        <v>73265</v>
+      </c>
+      <c r="J4" s="9">
+        <v>27357</v>
+      </c>
+      <c r="K4" s="9">
+        <v>22307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="9">
+        <v>476306</v>
+      </c>
+      <c r="G5" s="9">
+        <v>278848</v>
+      </c>
+      <c r="H5" s="9">
+        <v>51624</v>
+      </c>
+      <c r="I5" s="9">
+        <v>93727</v>
+      </c>
+      <c r="J5" s="9">
+        <v>21026</v>
+      </c>
+      <c r="K5" s="9">
+        <v>31081</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F6" s="9">
+        <v>547499</v>
+      </c>
+      <c r="G6" s="9">
+        <v>328920</v>
+      </c>
+      <c r="H6" s="9">
+        <v>61486</v>
+      </c>
+      <c r="I6" s="9">
+        <v>94697</v>
+      </c>
+      <c r="J6" s="9">
+        <v>33041</v>
+      </c>
+      <c r="K6" s="9">
+        <v>29355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F7" s="9">
+        <v>675353</v>
+      </c>
+      <c r="G7" s="9">
+        <v>401313</v>
+      </c>
+      <c r="H7" s="9">
+        <v>59789</v>
+      </c>
+      <c r="I7" s="9">
+        <v>145348</v>
+      </c>
+      <c r="J7" s="9">
+        <v>37375</v>
+      </c>
+      <c r="K7" s="9">
+        <v>31528</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" s="9">
+        <v>765859</v>
+      </c>
+      <c r="G8" s="9">
+        <v>433423.5</v>
+      </c>
+      <c r="H8" s="9">
+        <v>58720</v>
+      </c>
+      <c r="I8" s="9">
+        <v>183253.5</v>
+      </c>
+      <c r="J8" s="9">
+        <v>46778</v>
+      </c>
+      <c r="K8" s="9">
+        <v>43684</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>304</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" s="9">
+        <v>844950</v>
+      </c>
+      <c r="G9" s="9">
+        <v>477551</v>
+      </c>
+      <c r="H9" s="9">
+        <v>58436</v>
+      </c>
+      <c r="I9" s="9">
+        <v>204879</v>
+      </c>
+      <c r="J9" s="9">
+        <v>50432</v>
+      </c>
+      <c r="K9" s="9">
+        <v>53652</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>306</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F10" s="9">
+        <v>865572</v>
+      </c>
+      <c r="G10" s="9">
+        <v>504862</v>
+      </c>
+      <c r="H10" s="9">
+        <v>61040</v>
+      </c>
+      <c r="I10" s="9">
+        <v>195981</v>
+      </c>
+      <c r="J10" s="9">
+        <v>46781</v>
+      </c>
+      <c r="K10" s="9">
+        <v>56908</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>305</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C11" t="s">
+        <v>206</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F11" s="9">
+        <v>798455</v>
+      </c>
+      <c r="G11" s="9">
+        <v>470335</v>
+      </c>
+      <c r="H11" s="9">
+        <v>58790</v>
+      </c>
+      <c r="I11" s="9">
+        <v>168679</v>
+      </c>
+      <c r="J11" s="9">
+        <v>44147</v>
+      </c>
+      <c r="K11" s="9">
+        <v>56504</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F12" s="9">
+        <v>830441</v>
+      </c>
+      <c r="G12" s="9">
+        <v>476447</v>
+      </c>
+      <c r="H12" s="9">
+        <v>57645</v>
+      </c>
+      <c r="I12" s="9">
+        <v>194579</v>
+      </c>
+      <c r="J12" s="9">
+        <v>48984</v>
+      </c>
+      <c r="K12" s="9">
+        <v>52786</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>307</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F13" s="9">
+        <v>860441</v>
+      </c>
+      <c r="G13" s="9">
+        <v>492076</v>
+      </c>
+      <c r="H13" s="9">
+        <v>62425</v>
+      </c>
+      <c r="I13" s="9">
+        <v>212447</v>
+      </c>
+      <c r="J13" s="9">
+        <v>46739</v>
+      </c>
+      <c r="K13" s="9">
+        <v>46754</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>308</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" t="s">
+        <v>214</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F14" s="9">
+        <v>940000</v>
+      </c>
+      <c r="G14" s="9">
+        <v>569396</v>
+      </c>
+      <c r="H14" s="9">
+        <v>65418</v>
+      </c>
+      <c r="I14" s="9">
+        <v>198876</v>
+      </c>
+      <c r="J14" s="9">
+        <v>50819</v>
+      </c>
+      <c r="K14" s="9">
+        <v>55491</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>309</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F15" s="9">
+        <v>1066118</v>
+      </c>
+      <c r="G15" s="9">
+        <v>647335</v>
+      </c>
+      <c r="H15" s="9">
+        <v>71171</v>
+      </c>
+      <c r="I15" s="9">
+        <v>226185</v>
+      </c>
+      <c r="J15" s="9">
+        <v>60185</v>
+      </c>
+      <c r="K15" s="9">
+        <v>61242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>310</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C16" t="s">
+        <v>220</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F16" s="9">
+        <v>1253679</v>
+      </c>
+      <c r="G16" s="9">
+        <v>759187</v>
+      </c>
+      <c r="H16" s="9">
+        <v>102367</v>
+      </c>
+      <c r="I16" s="9">
+        <v>268631</v>
+      </c>
+      <c r="J16" s="9">
+        <v>60732</v>
+      </c>
+      <c r="K16" s="9">
+        <v>62762</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C17" t="s">
+        <v>224</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1456330</v>
+      </c>
+      <c r="G17" s="9">
+        <v>855773</v>
+      </c>
+      <c r="H17" s="9">
+        <v>124171</v>
+      </c>
+      <c r="I17" s="9">
+        <v>325738</v>
+      </c>
+      <c r="J17" s="9">
+        <v>72408</v>
+      </c>
+      <c r="K17" s="9">
+        <v>78240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>311</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C18" t="s">
+        <v>227</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F18" s="9">
+        <v>1425297</v>
+      </c>
+      <c r="G18" s="9">
+        <v>829759</v>
+      </c>
+      <c r="H18" s="9">
+        <v>124171</v>
+      </c>
+      <c r="I18" s="9">
+        <v>325738</v>
+      </c>
+      <c r="J18" s="9">
+        <v>72408</v>
+      </c>
+      <c r="K18" s="9">
+        <v>73221</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>228</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F19" s="9">
+        <v>1720846</v>
+      </c>
+      <c r="G19" s="9">
+        <v>1040477</v>
+      </c>
+      <c r="H19" s="9">
+        <v>140438</v>
+      </c>
+      <c r="I19" s="9">
+        <v>373831</v>
+      </c>
+      <c r="J19" s="9">
+        <v>79142</v>
+      </c>
+      <c r="K19" s="9">
+        <v>86958</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>232</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F20" s="9">
+        <v>1703946</v>
+      </c>
+      <c r="G20" s="9">
+        <v>1023577</v>
+      </c>
+      <c r="H20" s="9">
+        <v>140438</v>
+      </c>
+      <c r="I20" s="9">
+        <v>373831</v>
+      </c>
+      <c r="J20" s="9">
+        <v>79142</v>
+      </c>
+      <c r="K20" s="9">
+        <v>86958</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>312</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1673946</v>
+      </c>
+      <c r="G21" s="9">
+        <v>993577</v>
+      </c>
+      <c r="H21" s="9">
+        <v>140438</v>
+      </c>
+      <c r="I21" s="9">
+        <v>373831</v>
+      </c>
+      <c r="J21" s="9">
+        <v>79142</v>
+      </c>
+      <c r="K21" s="9">
+        <v>86958</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>313</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F22" s="9">
+        <v>2025664</v>
+      </c>
+      <c r="G22" s="9">
+        <v>1243401</v>
+      </c>
+      <c r="H22" s="9">
+        <v>170720</v>
+      </c>
+      <c r="I22" s="9">
+        <v>405111</v>
+      </c>
+      <c r="J22" s="9">
+        <v>82896</v>
+      </c>
+      <c r="K22" s="9">
+        <v>123536</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>314</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F23" s="9">
+        <v>1829248.5</v>
+      </c>
+      <c r="G23" s="9">
+        <v>1099740.8999999999</v>
+      </c>
+      <c r="H23" s="9">
+        <v>185028.6</v>
+      </c>
+      <c r="I23" s="9">
+        <v>364431.3</v>
+      </c>
+      <c r="J23" s="9">
+        <v>73346.2</v>
+      </c>
+      <c r="K23" s="9">
+        <v>106701.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>244</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F24" s="9">
+        <v>2039152</v>
+      </c>
+      <c r="G24" s="9">
+        <v>1045490.951</v>
+      </c>
+      <c r="H24" s="9">
+        <v>310208</v>
+      </c>
+      <c r="I24" s="9">
+        <v>456966.538</v>
+      </c>
+      <c r="J24" s="9">
+        <v>88535.603000000003</v>
+      </c>
+      <c r="K24" s="9">
+        <v>137950.908</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>315</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F25" s="9">
+        <v>2039152</v>
+      </c>
+      <c r="G25" s="9">
+        <v>1046538.95</v>
+      </c>
+      <c r="H25" s="9">
+        <v>309233</v>
+      </c>
+      <c r="I25" s="9">
+        <v>457284.53899999999</v>
+      </c>
+      <c r="J25" s="9">
+        <v>88341.603000000003</v>
+      </c>
+      <c r="K25" s="9">
+        <v>137753.908</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>250</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F26" s="9">
+        <v>2330693</v>
+      </c>
+      <c r="G26" s="9">
+        <v>1121867</v>
+      </c>
+      <c r="H26" s="9">
+        <v>400510</v>
+      </c>
+      <c r="I26" s="9">
+        <v>506825</v>
+      </c>
+      <c r="J26" s="9">
+        <v>112366</v>
+      </c>
+      <c r="K26" s="9">
+        <v>189125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>254</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F27" s="9">
+        <v>2271373</v>
+      </c>
+      <c r="G27" s="9">
+        <v>1157902</v>
+      </c>
+      <c r="H27" s="9">
+        <v>367799</v>
+      </c>
+      <c r="I27" s="9">
+        <v>423545</v>
+      </c>
+      <c r="J27" s="9">
+        <v>95091</v>
+      </c>
+      <c r="K27" s="9">
+        <v>227036</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>316</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F28" s="9">
+        <v>2330693</v>
+      </c>
+      <c r="G28" s="9">
+        <v>1121874</v>
+      </c>
+      <c r="H28" s="9">
+        <v>400510</v>
+      </c>
+      <c r="I28" s="9">
+        <v>506817</v>
+      </c>
+      <c r="J28" s="9">
+        <v>112367</v>
+      </c>
+      <c r="K28" s="9">
+        <v>189125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>259</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F29" s="9">
+        <v>2576003</v>
+      </c>
+      <c r="G29" s="9">
+        <v>1332915</v>
+      </c>
+      <c r="H29" s="9">
+        <v>464966</v>
+      </c>
+      <c r="I29" s="9">
+        <v>443900</v>
+      </c>
+      <c r="J29" s="9">
+        <v>108823</v>
+      </c>
+      <c r="K29" s="9">
+        <v>225399</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>263</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F30" s="9">
+        <v>2260484</v>
+      </c>
+      <c r="G30" s="9">
+        <v>1162225</v>
+      </c>
+      <c r="H30" s="9">
+        <v>364206</v>
+      </c>
+      <c r="I30" s="9">
+        <v>413336</v>
+      </c>
+      <c r="J30" s="9">
+        <v>137403</v>
+      </c>
+      <c r="K30" s="9">
+        <v>183314</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>266</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F31" s="9">
+        <v>1744104</v>
+      </c>
+      <c r="G31" s="9">
+        <v>937917</v>
+      </c>
+      <c r="H31" s="9">
+        <v>193757</v>
+      </c>
+      <c r="I31" s="9">
+        <v>340821</v>
+      </c>
+      <c r="J31" s="9">
+        <v>128030</v>
+      </c>
+      <c r="K31" s="9">
+        <v>143579</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>270</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="F32" s="9">
+        <v>1685734</v>
+      </c>
+      <c r="G32" s="9">
+        <v>786785</v>
+      </c>
+      <c r="H32" s="9">
+        <v>286576</v>
+      </c>
+      <c r="I32" s="9">
+        <v>350242</v>
+      </c>
+      <c r="J32" s="9">
+        <v>118699</v>
+      </c>
+      <c r="K32" s="9">
+        <v>143432</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>320</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F33" s="9">
+        <v>1685734</v>
+      </c>
+      <c r="G33" s="9">
+        <v>786785</v>
+      </c>
+      <c r="H33" s="9">
+        <v>286576</v>
+      </c>
+      <c r="I33" s="9">
+        <v>350242</v>
+      </c>
+      <c r="J33" s="9">
+        <v>118699</v>
+      </c>
+      <c r="K33" s="9">
+        <v>143432</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>273</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F34" s="9">
+        <v>2081161</v>
+      </c>
+      <c r="G34" s="9">
+        <v>1032952</v>
+      </c>
+      <c r="H34" s="9">
+        <v>332102</v>
+      </c>
+      <c r="I34" s="9">
+        <v>405250</v>
+      </c>
+      <c r="J34" s="9">
+        <v>129292</v>
+      </c>
+      <c r="K34" s="9">
+        <v>181565</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>321</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C35" t="s">
+        <v>277</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F35" s="9">
+        <v>2081161</v>
+      </c>
+      <c r="G35" s="9">
+        <f>1015431+39712</f>
+        <v>1055143</v>
+      </c>
+      <c r="H35" s="9">
+        <v>305218</v>
+      </c>
+      <c r="I35" s="9">
+        <v>378721</v>
+      </c>
+      <c r="J35" s="9">
+        <v>127860</v>
+      </c>
+      <c r="K35" s="9">
+        <v>214219</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>278</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F36" s="9">
+        <v>2438302</v>
+      </c>
+      <c r="G36" s="9">
+        <v>1225218.0830000001</v>
+      </c>
+      <c r="H36" s="9">
+        <v>348345</v>
+      </c>
+      <c r="I36" s="9">
+        <v>501631.55300000001</v>
+      </c>
+      <c r="J36" s="9">
+        <v>136741.364</v>
+      </c>
+      <c r="K36" s="9">
+        <v>226366</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>282</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F37" s="9">
+        <v>2438302</v>
+      </c>
+      <c r="G37" s="9">
+        <v>1225218.0830000001</v>
+      </c>
+      <c r="H37" s="9">
+        <v>348345</v>
+      </c>
+      <c r="I37" s="9">
+        <v>501631.55300000001</v>
+      </c>
+      <c r="J37" s="9">
+        <v>136741.364</v>
+      </c>
+      <c r="K37" s="9">
+        <v>226366</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>322</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F38" s="9">
+        <v>2392587</v>
+      </c>
+      <c r="G38" s="9">
+        <v>1197966</v>
+      </c>
+      <c r="H38" s="9">
+        <v>365197</v>
+      </c>
+      <c r="I38" s="9">
+        <v>430160.55300000001</v>
+      </c>
+      <c r="J38" s="9">
+        <v>153695.364</v>
+      </c>
+      <c r="K38" s="9">
+        <v>245568</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>287</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F39" s="9">
+        <v>2599127</v>
+      </c>
+      <c r="G39" s="9">
+        <v>1368921</v>
+      </c>
+      <c r="H39" s="9">
+        <v>352876</v>
+      </c>
+      <c r="I39" s="9">
+        <v>507027</v>
+      </c>
+      <c r="J39" s="9">
+        <v>125049</v>
+      </c>
+      <c r="K39" s="9">
+        <f>230480+14774</f>
+        <v>245254</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>290</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F40" s="9">
+        <v>2639174</v>
+      </c>
+      <c r="G40" s="9">
+        <v>1397523</v>
+      </c>
+      <c r="H40" s="9">
+        <v>336093</v>
+      </c>
+      <c r="I40" s="9">
+        <v>538131</v>
+      </c>
+      <c r="J40" s="9">
+        <v>124646</v>
+      </c>
+      <c r="K40" s="9">
+        <v>242781</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F41" s="9">
+        <v>2639174</v>
+      </c>
+      <c r="G41" s="9">
+        <f>1316452+81071</f>
+        <v>1397523</v>
+      </c>
+      <c r="H41" s="9">
+        <v>336093</v>
+      </c>
+      <c r="I41" s="9">
+        <v>538131</v>
+      </c>
+      <c r="J41" s="9">
+        <v>124646</v>
+      </c>
+      <c r="K41" s="9">
+        <f>224154+18627</f>
+        <v>242781</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>295</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F42" s="9">
+        <v>3055169</v>
+      </c>
+      <c r="G42" s="9">
+        <f>1649267+72127</f>
+        <v>1721394</v>
+      </c>
+      <c r="H42" s="9">
+        <v>326195</v>
+      </c>
+      <c r="I42" s="9">
+        <v>599235</v>
+      </c>
+      <c r="J42" s="9">
+        <v>163216</v>
+      </c>
+      <c r="K42" s="9">
+        <f>229242+15887</f>
+        <v>245129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>299</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F43" s="9">
+        <v>3046751.2749999999</v>
+      </c>
+      <c r="G43" s="9">
+        <f>1467398.307+ 85227.022</f>
+        <v>1552625.3289999999</v>
+      </c>
+      <c r="H43" s="9">
+        <v>457812.31400000001</v>
+      </c>
+      <c r="I43" s="9">
+        <v>620708.23899999994</v>
+      </c>
+      <c r="J43" s="9">
+        <v>144379.228</v>
+      </c>
+      <c r="K43" s="9">
+        <f>255339.165+ 15887</f>
+        <v>271226.16500000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9433,7 +11502,7 @@
         <v>140</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -9449,49 +11518,62 @@
         <v>144</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" t="s">
         <v>146</v>
-      </c>
-      <c r="B13" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
+      <c r="B14" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="4" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>149</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>150</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>151</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>152</v>
+      <c r="A18" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9500,8 +11582,9 @@
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="B17" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="B18" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B19" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B20" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B14" r:id="rId5" xr:uid="{437668B8-5186-42B0-A692-8F19A10F67FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>